<commit_message>
Fixed the whole_ex2 + typos in the header
</commit_message>
<xml_diff>
--- a/data/transcriptions/template.xlsx
+++ b/data/transcriptions/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/seorin_kim_vub_be/Documents/img-analysis_seorin_project/data/transcriptions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serenekim/Desktop/PhD/img-analysis_seorin_project/data/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EFBA3DE7-74C1-D743-9CDA-187428393E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CE0D89A-40EB-9543-BE30-852F4F109A16}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE17E00-11AC-124D-BFF0-64BC813C9645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18400" yWindow="760" windowWidth="11840" windowHeight="18880" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
   </bookViews>
@@ -107,9 +107,6 @@
     <t>Observations</t>
   </si>
   <si>
-    <t>(les déclarations qui figurent à l'état n'413 doivent être émargées en conséquence, dans la présnete colonne.)</t>
-  </si>
-  <si>
     <t>Droit de mutation par déces</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>N' d'ordre</t>
+  </si>
+  <si>
+    <t>(les déclarations qui figurent à l'état n'413 doivent être émargées en conséquence, dans la présente colonne.)</t>
   </si>
 </sst>
 </file>
@@ -716,15 +716,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB076F5B-4564-1543-8968-7E29FE54F40E}">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="236" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:21" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>4</v>
@@ -747,7 +747,7 @@
       <c r="J1" s="32"/>
       <c r="K1" s="29"/>
       <c r="L1" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M1" s="28" t="s">
         <v>11</v>
@@ -796,7 +796,7 @@
         <v>10</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" s="17" t="s">
         <v>12</v>
@@ -821,7 +821,7 @@
         <v>21</v>
       </c>
       <c r="U2" s="13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="14" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>